<commit_message>
crop segmentation and ave_ref
</commit_message>
<xml_diff>
--- a/appf_toolbox_structure.xlsx
+++ b/appf_toolbox_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t xml:space="preserve">f: function; c: class; p: pending work</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t xml:space="preserve">spectral_resample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crop_segmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ave_ref_crop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f, average the reflectance of crops</t>
   </si>
   <si>
     <t xml:space="preserve">transformation.py</t>
@@ -216,10 +225,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F29"/>
+  <dimension ref="B1:F31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,48 +334,48 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="F16" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>6</v>
-      </c>
+      <c r="D18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -374,7 +383,7 @@
       <c r="D22" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="0" t="s">
@@ -382,16 +391,16 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="E24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>6</v>
@@ -399,7 +408,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>6</v>
@@ -407,7 +416,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>6</v>
@@ -415,7 +424,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>6</v>
@@ -423,7 +432,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>6</v>
@@ -431,9 +440,25 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F29" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The version of APPF_toolbox_private
</commit_message>
<xml_diff>
--- a/appf_toolbox_structure.xlsx
+++ b/appf_toolbox_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python_projects\appf_toolbox_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334E5B5E-A8BF-45B2-B06D-FF2FB8FD38D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16742F5F-69DF-4918-A15C-02389C540E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>f: function; c: class; p: pending work</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>fuse_fx17_to_fx10</t>
+  </si>
+  <si>
+    <t>first_order_derivative</t>
+  </si>
+  <si>
+    <t>second_order_derivative</t>
   </si>
 </sst>
 </file>
@@ -538,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F45"/>
+  <dimension ref="B1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -709,43 +715,43 @@
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>30</v>
+      <c r="E25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
         <v>31</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>32</v>
-      </c>
-      <c r="F26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>34</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -753,7 +759,7 @@
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -761,7 +767,7 @@
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -769,7 +775,7 @@
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -777,7 +783,7 @@
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -785,18 +791,15 @@
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
-        <v>40</v>
-      </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -804,15 +807,18 @@
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -820,76 +826,92 @@
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
         <v>43</v>
       </c>
-      <c r="F37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E40" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" t="s">
-        <v>2</v>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
         <v>50</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E45" t="s">
         <v>51</v>
       </c>
-      <c r="F43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E44" t="s">
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
         <v>52</v>
       </c>
-      <c r="F44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E45" t="s">
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
         <v>53</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F47" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>